<commit_message>
Update requisitos/Requisitos.xlsx: fix typo R31
</commit_message>
<xml_diff>
--- a/requisitos/Requisitos.xlsx
+++ b/requisitos/Requisitos.xlsx
@@ -45,7 +45,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="98">
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
   <si>
     <t>Consultoria de Detetives Christie</t>
   </si>
@@ -235,7 +238,7 @@
     <t>Devido a natureza do relacionamento entre suspeitos e casos (N:M) é feito um mapeamento entre os identificadores de caso e de suspeito.</t>
   </si>
   <si>
-    <t>Um registo de uma vinculação efetua a ligação entre um caso e os seus detetives, e deve incluir os seguintes atributos: data de vinculação, data de desvinculção (opcional) e descrição.</t>
+    <t>Um registo de uma vinculação efetua a ligação entre um caso e os seus detetives, e deve incluir os seguintes atributos: data de vinculação, data de desvinculação (opcional) e descrição.</t>
   </si>
   <si>
     <t>Vinculações</t>
@@ -385,6 +388,9 @@
   </si>
   <si>
     <t>Todos os casos têm associado um único cliente.</t>
+  </si>
+  <si>
+    <t>Um registo de uma vinculação efetua a ligação entre um caso e os seus detetives, e deve incluir os seguintes atributos: data de vinculação, data de desvinculção (opcional) e descrição.</t>
   </si>
   <si>
     <r>
@@ -653,11 +659,13 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -711,6 +719,7 @@
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -718,6 +727,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -975,16 +987,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A9:F36" displayName="Table_2" name="Table_2" id="2">
-  <tableColumns count="6">
-    <tableColumn name="Nr" id="1"/>
-    <tableColumn name="Data e Hora" id="2"/>
-    <tableColumn name="Descrição" id="3"/>
-    <tableColumn name="Área" id="4"/>
-    <tableColumn name="Fonte" id="5"/>
-    <tableColumn name="Analista" id="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A9:G36" displayName="Table_2" name="Table_2" id="2">
+  <tableColumns count="7">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+    <tableColumn name="Column5" id="5"/>
+    <tableColumn name="Column6" id="6"/>
+    <tableColumn name="Column7" id="7"/>
   </tableColumns>
   <tableStyleInfo name="Requisitos de Descrição-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
+    </ext>
+  </extLst>
 </table>
 </file>
 
@@ -1247,34 +1265,36 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1"/>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1"/>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E7" s="7">
         <v>45376.0</v>
@@ -1283,25 +1303,25 @@
     <row r="8" ht="15.75" customHeight="1"/>
     <row r="9" ht="22.5" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
@@ -1312,19 +1332,19 @@
         <v>45371.75347222222</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
@@ -1335,19 +1355,19 @@
         <v>45371.75347222222</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
@@ -1358,19 +1378,19 @@
         <v>45361.38888888889</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
@@ -1381,19 +1401,19 @@
         <v>45376.90277777778</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>20</v>
-      </c>
       <c r="F13" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
@@ -1404,19 +1424,19 @@
         <v>45361.39027777778</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
@@ -1427,19 +1447,19 @@
         <v>45371.76736111111</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
@@ -1450,19 +1470,19 @@
         <v>45371.76736111111</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
@@ -1473,19 +1493,19 @@
         <v>45371.76736111111</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
@@ -1496,19 +1516,19 @@
         <v>45371.76736111111</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
@@ -1519,19 +1539,19 @@
         <v>45371.76736111111</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
@@ -1542,19 +1562,19 @@
         <v>45371.75486111111</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -1565,19 +1585,19 @@
         <v>45363.819444444445</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
@@ -1588,19 +1608,19 @@
         <v>45376.90972222222</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -1611,19 +1631,19 @@
         <v>45371.77777777778</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
@@ -1634,19 +1654,19 @@
         <v>45361.430555555555</v>
       </c>
       <c r="C24" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="E24" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H24" s="15"/>
     </row>
@@ -1658,19 +1678,19 @@
         <v>45371.76736111111</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -1681,19 +1701,19 @@
         <v>45361.44583333333</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
@@ -1704,19 +1724,19 @@
         <v>45371.76736111111</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
@@ -1727,19 +1747,19 @@
         <v>45371.774305555555</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
@@ -1750,19 +1770,19 @@
         <v>45361.54861111111</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
@@ -1773,19 +1793,19 @@
         <v>45371.770833333336</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
@@ -1796,19 +1816,19 @@
         <v>45361.52638888889</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
@@ -1819,19 +1839,19 @@
         <v>45361.52569444444</v>
       </c>
       <c r="C32" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="E32" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
@@ -1842,19 +1862,19 @@
         <v>45361.527083333334</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
@@ -1865,19 +1885,19 @@
         <v>45361.458333333336</v>
       </c>
       <c r="C34" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="10" t="s">
-        <v>47</v>
-      </c>
       <c r="E34" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
@@ -1888,19 +1908,19 @@
         <v>45361.555555555555</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
@@ -1911,19 +1931,19 @@
         <v>45361.52777777778</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
@@ -1934,19 +1954,19 @@
         <v>45361.459027777775</v>
       </c>
       <c r="C37" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="10" t="s">
-        <v>51</v>
-      </c>
       <c r="E37" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
@@ -1957,19 +1977,19 @@
         <v>45376.90625</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
@@ -1980,19 +2000,19 @@
         <v>45361.55902777778</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
@@ -2003,19 +2023,19 @@
         <v>45361.520833333336</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
@@ -2026,19 +2046,19 @@
         <v>45361.524305555555</v>
       </c>
       <c r="C41" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D41" s="10" t="s">
-        <v>56</v>
-      </c>
       <c r="E41" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
@@ -2049,19 +2069,19 @@
         <v>45361.53472222222</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
@@ -2072,19 +2092,19 @@
         <v>45361.53472222222</v>
       </c>
       <c r="C43" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D43" s="10" t="s">
-        <v>59</v>
-      </c>
       <c r="E43" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
@@ -2095,19 +2115,19 @@
         <v>45361.53958333333</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
@@ -2118,19 +2138,19 @@
         <v>45361.540972222225</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
@@ -2141,19 +2161,19 @@
         <v>45376.90625</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -2164,19 +2184,19 @@
         <v>45362.84027777778</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
@@ -2187,19 +2207,19 @@
         <v>45361.47222222222</v>
       </c>
       <c r="C48" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G48" s="10" t="s">
         <v>67</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F48" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G48" s="10" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
@@ -2210,19 +2230,19 @@
         <v>45371.774305555555</v>
       </c>
       <c r="C49" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D49" s="10" t="s">
-        <v>68</v>
-      </c>
       <c r="E49" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
@@ -2233,19 +2253,19 @@
         <v>45362.83472222222</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
@@ -2256,19 +2276,19 @@
         <v>45362.836805555555</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
@@ -2279,19 +2299,19 @@
         <v>45361.68402777778</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
@@ -2302,19 +2322,19 @@
         <v>45361.68402777778</v>
       </c>
       <c r="C53" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D53" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D53" s="10" t="s">
-        <v>73</v>
-      </c>
       <c r="E53" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
@@ -2325,19 +2345,19 @@
         <v>45361.68472222222</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
@@ -2348,19 +2368,19 @@
         <v>45361.694444444445</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
@@ -2371,19 +2391,19 @@
         <v>45361.70138888889</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
@@ -2394,19 +2414,19 @@
         <v>45362.819444444445</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
@@ -2417,19 +2437,19 @@
         <v>45371.77777777778</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
@@ -2524,38 +2544,38 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="24" t="s">
-        <v>80</v>
+      <c r="A1" s="23"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="25" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1"/>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1"/>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="25" t="s">
-        <v>81</v>
+      <c r="A7" s="26" t="s">
+        <v>82</v>
       </c>
       <c r="E7" s="7">
         <v>45376.0</v>
@@ -2564,23 +2584,24 @@
     <row r="8" ht="15.75" customHeight="1"/>
     <row r="9" ht="22.5" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="10">
@@ -2590,16 +2611,16 @@
         <v>45371.75347222222</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G10" s="10"/>
     </row>
@@ -2611,16 +2632,16 @@
         <v>45371.75347222222</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G11" s="10"/>
     </row>
@@ -2632,16 +2653,16 @@
         <v>45361.38888888889</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G12" s="10"/>
     </row>
@@ -2653,16 +2674,16 @@
         <v>45376.90277777778</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>20</v>
-      </c>
       <c r="F13" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G13" s="10"/>
     </row>
@@ -2674,16 +2695,16 @@
         <v>45371.76736111111</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G14" s="10"/>
     </row>
@@ -2695,16 +2716,16 @@
         <v>45371.76736111111</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G15" s="10"/>
     </row>
@@ -2716,16 +2737,16 @@
         <v>45371.76736111111</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G16" s="10"/>
     </row>
@@ -2737,16 +2758,16 @@
         <v>45371.76736111111</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G17" s="10"/>
     </row>
@@ -2758,16 +2779,16 @@
         <v>45371.76736111111</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G18" s="10"/>
     </row>
@@ -2779,16 +2800,16 @@
         <v>45371.77777777778</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G19" s="10"/>
     </row>
@@ -2800,16 +2821,16 @@
         <v>45361.430555555555</v>
       </c>
       <c r="C20" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="E20" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G20" s="10"/>
       <c r="H20" s="15"/>
@@ -2822,16 +2843,16 @@
         <v>45371.76736111111</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G21" s="10"/>
     </row>
@@ -2843,16 +2864,16 @@
         <v>45361.44583333333</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G22" s="10"/>
     </row>
@@ -2864,16 +2885,16 @@
         <v>45371.76736111111</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G23" s="10"/>
     </row>
@@ -2885,16 +2906,16 @@
         <v>45361.52638888889</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G24" s="10"/>
     </row>
@@ -2906,16 +2927,16 @@
         <v>45361.52569444444</v>
       </c>
       <c r="C25" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="E25" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G25" s="10"/>
     </row>
@@ -2927,16 +2948,16 @@
         <v>45361.527083333334</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G26" s="10"/>
     </row>
@@ -2948,16 +2969,16 @@
         <v>45361.458333333336</v>
       </c>
       <c r="C27" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>47</v>
-      </c>
       <c r="E27" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G27" s="10"/>
     </row>
@@ -2969,16 +2990,16 @@
         <v>45361.555555555555</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G28" s="10"/>
     </row>
@@ -2990,16 +3011,16 @@
         <v>45361.52777777778</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G29" s="10"/>
     </row>
@@ -3011,16 +3032,16 @@
         <v>45361.459027777775</v>
       </c>
       <c r="C30" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="10" t="s">
-        <v>51</v>
-      </c>
       <c r="E30" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G30" s="10"/>
     </row>
@@ -3032,16 +3053,16 @@
         <v>45376.90625</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G31" s="10"/>
     </row>
@@ -3053,16 +3074,16 @@
         <v>45361.55902777778</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G32" s="10"/>
     </row>
@@ -3074,16 +3095,16 @@
         <v>45361.520833333336</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G33" s="10"/>
     </row>
@@ -3095,16 +3116,16 @@
         <v>45361.53472222222</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G34" s="10"/>
     </row>
@@ -3116,16 +3137,16 @@
         <v>45361.53472222222</v>
       </c>
       <c r="C35" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D35" s="10" t="s">
-        <v>59</v>
-      </c>
       <c r="E35" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G35" s="10"/>
     </row>
@@ -3137,37 +3158,37 @@
         <v>45361.53958333333</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G36" s="10"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="26">
+      <c r="A37" s="28">
         <v>36.0</v>
       </c>
-      <c r="B37" s="27">
+      <c r="B37" s="29">
         <v>45361.540972222225</v>
       </c>
-      <c r="C37" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="D37" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="E37" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="F37" s="26" t="s">
-        <v>18</v>
+      <c r="C37" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F37" s="28" t="s">
+        <v>19</v>
       </c>
       <c r="G37" s="10"/>
     </row>
@@ -3179,16 +3200,16 @@
         <v>45376.90625</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G38" s="10"/>
     </row>
@@ -3264,37 +3285,37 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1"/>
-      <c r="F1" s="28" t="s">
-        <v>85</v>
+      <c r="A1" s="23"/>
+      <c r="F1" s="30" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1"/>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1"/>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="29" t="s">
-        <v>86</v>
+      <c r="A7" s="31" t="s">
+        <v>88</v>
       </c>
       <c r="E7" s="7">
         <v>45376.0</v>
@@ -3303,739 +3324,739 @@
     <row r="8" ht="15.75" customHeight="1"/>
     <row r="9" ht="22.5" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="30"/>
-      <c r="T9" s="30"/>
-      <c r="U9" s="30"/>
-      <c r="V9" s="30"/>
-      <c r="W9" s="30"/>
-      <c r="X9" s="30"/>
-      <c r="Y9" s="30"/>
-      <c r="Z9" s="30"/>
+        <v>12</v>
+      </c>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="32"/>
+      <c r="V9" s="32"/>
+      <c r="W9" s="32"/>
+      <c r="X9" s="32"/>
+      <c r="Y9" s="32"/>
+      <c r="Z9" s="32"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="31">
+      <c r="A10" s="33">
         <v>5.0</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="34">
         <v>45361.39027777778</v>
       </c>
-      <c r="C10" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="34"/>
-      <c r="R10" s="34"/>
-      <c r="S10" s="34"/>
-      <c r="T10" s="34"/>
-      <c r="U10" s="34"/>
-      <c r="V10" s="34"/>
-      <c r="W10" s="34"/>
-      <c r="X10" s="34"/>
-      <c r="Y10" s="34"/>
-      <c r="Z10" s="34"/>
+      <c r="C10" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="36"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="36"/>
+      <c r="Q10" s="36"/>
+      <c r="R10" s="36"/>
+      <c r="S10" s="36"/>
+      <c r="T10" s="36"/>
+      <c r="U10" s="36"/>
+      <c r="V10" s="36"/>
+      <c r="W10" s="36"/>
+      <c r="X10" s="36"/>
+      <c r="Y10" s="36"/>
+      <c r="Z10" s="36"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="36">
+      <c r="A11" s="38">
         <v>11.0</v>
       </c>
-      <c r="B11" s="37">
+      <c r="B11" s="39">
         <v>45371.75486111111</v>
       </c>
-      <c r="C11" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="39" t="s">
+      <c r="C11" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
-      <c r="P11" s="34"/>
-      <c r="Q11" s="34"/>
-      <c r="R11" s="34"/>
-      <c r="S11" s="34"/>
-      <c r="T11" s="34"/>
-      <c r="U11" s="34"/>
-      <c r="V11" s="34"/>
-      <c r="W11" s="34"/>
-      <c r="X11" s="34"/>
-      <c r="Y11" s="34"/>
-      <c r="Z11" s="34"/>
+      <c r="D11" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="36"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="36"/>
+      <c r="Q11" s="36"/>
+      <c r="R11" s="36"/>
+      <c r="S11" s="36"/>
+      <c r="T11" s="36"/>
+      <c r="U11" s="36"/>
+      <c r="V11" s="36"/>
+      <c r="W11" s="36"/>
+      <c r="X11" s="36"/>
+      <c r="Y11" s="36"/>
+      <c r="Z11" s="36"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="40">
+      <c r="A12" s="42">
         <v>12.0</v>
       </c>
-      <c r="B12" s="41">
+      <c r="B12" s="43">
         <v>45363.819444444445</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="36"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="36"/>
+      <c r="R12" s="36"/>
+      <c r="S12" s="36"/>
+      <c r="T12" s="36"/>
+      <c r="U12" s="36"/>
+      <c r="V12" s="36"/>
+      <c r="W12" s="36"/>
+      <c r="X12" s="36"/>
+      <c r="Y12" s="36"/>
+      <c r="Z12" s="36"/>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="38">
+        <v>13.0</v>
+      </c>
+      <c r="B13" s="39">
+        <v>45376.90972222222</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="34"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="34"/>
-      <c r="P12" s="34"/>
-      <c r="Q12" s="34"/>
-      <c r="R12" s="34"/>
-      <c r="S12" s="34"/>
-      <c r="T12" s="34"/>
-      <c r="U12" s="34"/>
-      <c r="V12" s="34"/>
-      <c r="W12" s="34"/>
-      <c r="X12" s="34"/>
-      <c r="Y12" s="34"/>
-      <c r="Z12" s="34"/>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="36">
-        <v>13.0</v>
-      </c>
-      <c r="B13" s="37">
-        <v>45376.90972222222</v>
-      </c>
-      <c r="C13" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="34"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="34"/>
-      <c r="Q13" s="34"/>
-      <c r="R13" s="34"/>
-      <c r="S13" s="34"/>
-      <c r="T13" s="34"/>
-      <c r="U13" s="34"/>
-      <c r="V13" s="34"/>
-      <c r="W13" s="34"/>
-      <c r="X13" s="34"/>
-      <c r="Y13" s="34"/>
-      <c r="Z13" s="34"/>
+      <c r="F13" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="36"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="36"/>
+      <c r="S13" s="36"/>
+      <c r="T13" s="36"/>
+      <c r="U13" s="36"/>
+      <c r="V13" s="36"/>
+      <c r="W13" s="36"/>
+      <c r="X13" s="36"/>
+      <c r="Y13" s="36"/>
+      <c r="Z13" s="36"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="31">
+      <c r="A14" s="33">
         <v>19.0</v>
       </c>
-      <c r="B14" s="32">
+      <c r="B14" s="34">
         <v>45371.774305555555</v>
       </c>
-      <c r="C14" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="34"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="34"/>
-      <c r="P14" s="34"/>
-      <c r="Q14" s="34"/>
-      <c r="R14" s="34"/>
-      <c r="S14" s="34"/>
-      <c r="T14" s="34"/>
-      <c r="U14" s="34"/>
-      <c r="V14" s="34"/>
-      <c r="W14" s="34"/>
-      <c r="X14" s="34"/>
-      <c r="Y14" s="34"/>
-      <c r="Z14" s="34"/>
+      <c r="C14" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="36"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="36"/>
+      <c r="S14" s="36"/>
+      <c r="T14" s="36"/>
+      <c r="U14" s="36"/>
+      <c r="V14" s="36"/>
+      <c r="W14" s="36"/>
+      <c r="X14" s="36"/>
+      <c r="Y14" s="36"/>
+      <c r="Z14" s="36"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="36">
+      <c r="A15" s="38">
         <v>20.0</v>
       </c>
-      <c r="B15" s="37">
+      <c r="B15" s="39">
         <v>45361.54861111111</v>
       </c>
-      <c r="C15" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="34"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
-      <c r="P15" s="34"/>
-      <c r="Q15" s="34"/>
-      <c r="R15" s="34"/>
-      <c r="S15" s="34"/>
-      <c r="T15" s="34"/>
-      <c r="U15" s="34"/>
-      <c r="V15" s="34"/>
-      <c r="W15" s="34"/>
-      <c r="X15" s="34"/>
-      <c r="Y15" s="34"/>
-      <c r="Z15" s="34"/>
+      <c r="C15" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="36"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="36"/>
+      <c r="S15" s="36"/>
+      <c r="T15" s="36"/>
+      <c r="U15" s="36"/>
+      <c r="V15" s="36"/>
+      <c r="W15" s="36"/>
+      <c r="X15" s="36"/>
+      <c r="Y15" s="36"/>
+      <c r="Z15" s="36"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="31">
+      <c r="A16" s="33">
         <v>21.0</v>
       </c>
-      <c r="B16" s="32">
+      <c r="B16" s="34">
         <v>45371.770833333336</v>
       </c>
-      <c r="C16" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="33" t="s">
+      <c r="C16" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="36"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="36"/>
+      <c r="S16" s="36"/>
+      <c r="T16" s="36"/>
+      <c r="U16" s="36"/>
+      <c r="V16" s="36"/>
+      <c r="W16" s="36"/>
+      <c r="X16" s="36"/>
+      <c r="Y16" s="36"/>
+      <c r="Z16" s="36"/>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="38">
+        <v>32.0</v>
+      </c>
+      <c r="B17" s="39">
+        <v>45361.524305555555</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="36"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="36"/>
+      <c r="R17" s="36"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="36"/>
+      <c r="U17" s="36"/>
+      <c r="V17" s="36"/>
+      <c r="W17" s="36"/>
+      <c r="X17" s="36"/>
+      <c r="Y17" s="36"/>
+      <c r="Z17" s="36"/>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="33">
+        <v>41.0</v>
+      </c>
+      <c r="B18" s="34">
+        <v>45362.836805555555</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="36"/>
+      <c r="T18" s="36"/>
+      <c r="U18" s="36"/>
+      <c r="V18" s="36"/>
+      <c r="W18" s="36"/>
+      <c r="X18" s="36"/>
+      <c r="Y18" s="36"/>
+      <c r="Z18" s="36"/>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="38">
+        <v>42.0</v>
+      </c>
+      <c r="B19" s="39">
+        <v>45361.68402777778</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="36"/>
+      <c r="R19" s="36"/>
+      <c r="S19" s="36"/>
+      <c r="T19" s="36"/>
+      <c r="U19" s="36"/>
+      <c r="V19" s="36"/>
+      <c r="W19" s="36"/>
+      <c r="X19" s="36"/>
+      <c r="Y19" s="36"/>
+      <c r="Z19" s="36"/>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="33">
+        <v>43.0</v>
+      </c>
+      <c r="B20" s="34">
+        <v>45361.68402777778</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="36"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="36"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="36"/>
+      <c r="Q20" s="36"/>
+      <c r="R20" s="36"/>
+      <c r="S20" s="36"/>
+      <c r="T20" s="36"/>
+      <c r="U20" s="36"/>
+      <c r="V20" s="36"/>
+      <c r="W20" s="36"/>
+      <c r="X20" s="36"/>
+      <c r="Y20" s="36"/>
+      <c r="Z20" s="36"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="38">
+        <v>44.0</v>
+      </c>
+      <c r="B21" s="39">
+        <v>45361.68472222222</v>
+      </c>
+      <c r="C21" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="36"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="36"/>
+      <c r="R21" s="36"/>
+      <c r="S21" s="36"/>
+      <c r="T21" s="36"/>
+      <c r="U21" s="36"/>
+      <c r="V21" s="36"/>
+      <c r="W21" s="36"/>
+      <c r="X21" s="36"/>
+      <c r="Y21" s="36"/>
+      <c r="Z21" s="36"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="33">
+        <v>45.0</v>
+      </c>
+      <c r="B22" s="34">
+        <v>45361.694444444445</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="36"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="36"/>
+      <c r="R22" s="36"/>
+      <c r="S22" s="36"/>
+      <c r="T22" s="36"/>
+      <c r="U22" s="36"/>
+      <c r="V22" s="36"/>
+      <c r="W22" s="36"/>
+      <c r="X22" s="36"/>
+      <c r="Y22" s="36"/>
+      <c r="Z22" s="36"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="38">
+        <v>46.0</v>
+      </c>
+      <c r="B23" s="39">
+        <v>45361.70138888889</v>
+      </c>
+      <c r="C23" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="36"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="36"/>
+      <c r="O23" s="36"/>
+      <c r="P23" s="36"/>
+      <c r="Q23" s="36"/>
+      <c r="R23" s="36"/>
+      <c r="S23" s="36"/>
+      <c r="T23" s="36"/>
+      <c r="U23" s="36"/>
+      <c r="V23" s="36"/>
+      <c r="W23" s="36"/>
+      <c r="X23" s="36"/>
+      <c r="Y23" s="36"/>
+      <c r="Z23" s="36"/>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="33">
+        <v>47.0</v>
+      </c>
+      <c r="B24" s="34">
+        <v>45362.819444444445</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="36"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="36"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="36"/>
+      <c r="Q24" s="36"/>
+      <c r="R24" s="36"/>
+      <c r="S24" s="36"/>
+      <c r="T24" s="36"/>
+      <c r="U24" s="36"/>
+      <c r="V24" s="36"/>
+      <c r="W24" s="36"/>
+      <c r="X24" s="36"/>
+      <c r="Y24" s="36"/>
+      <c r="Z24" s="36"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="38">
+        <v>48.0</v>
+      </c>
+      <c r="B25" s="39">
+        <v>45371.77777777778</v>
+      </c>
+      <c r="C25" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="34"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="34"/>
-      <c r="P16" s="34"/>
-      <c r="Q16" s="34"/>
-      <c r="R16" s="34"/>
-      <c r="S16" s="34"/>
-      <c r="T16" s="34"/>
-      <c r="U16" s="34"/>
-      <c r="V16" s="34"/>
-      <c r="W16" s="34"/>
-      <c r="X16" s="34"/>
-      <c r="Y16" s="34"/>
-      <c r="Z16" s="34"/>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="36">
-        <v>32.0</v>
-      </c>
-      <c r="B17" s="37">
-        <v>45361.524305555555</v>
-      </c>
-      <c r="C17" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="34"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="34"/>
-      <c r="P17" s="34"/>
-      <c r="Q17" s="34"/>
-      <c r="R17" s="34"/>
-      <c r="S17" s="34"/>
-      <c r="T17" s="34"/>
-      <c r="U17" s="34"/>
-      <c r="V17" s="34"/>
-      <c r="W17" s="34"/>
-      <c r="X17" s="34"/>
-      <c r="Y17" s="34"/>
-      <c r="Z17" s="34"/>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="31">
-        <v>41.0</v>
-      </c>
-      <c r="B18" s="32">
-        <v>45362.836805555555</v>
-      </c>
-      <c r="C18" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="34"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="34"/>
-      <c r="O18" s="34"/>
-      <c r="P18" s="34"/>
-      <c r="Q18" s="34"/>
-      <c r="R18" s="34"/>
-      <c r="S18" s="34"/>
-      <c r="T18" s="34"/>
-      <c r="U18" s="34"/>
-      <c r="V18" s="34"/>
-      <c r="W18" s="34"/>
-      <c r="X18" s="34"/>
-      <c r="Y18" s="34"/>
-      <c r="Z18" s="34"/>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="36">
-        <v>42.0</v>
-      </c>
-      <c r="B19" s="37">
-        <v>45361.68402777778</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="34"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="34"/>
-      <c r="P19" s="34"/>
-      <c r="Q19" s="34"/>
-      <c r="R19" s="34"/>
-      <c r="S19" s="34"/>
-      <c r="T19" s="34"/>
-      <c r="U19" s="34"/>
-      <c r="V19" s="34"/>
-      <c r="W19" s="34"/>
-      <c r="X19" s="34"/>
-      <c r="Y19" s="34"/>
-      <c r="Z19" s="34"/>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="31">
-        <v>43.0</v>
-      </c>
-      <c r="B20" s="32">
-        <v>45361.68402777778</v>
-      </c>
-      <c r="C20" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="34"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="34"/>
-      <c r="Q20" s="34"/>
-      <c r="R20" s="34"/>
-      <c r="S20" s="34"/>
-      <c r="T20" s="34"/>
-      <c r="U20" s="34"/>
-      <c r="V20" s="34"/>
-      <c r="W20" s="34"/>
-      <c r="X20" s="34"/>
-      <c r="Y20" s="34"/>
-      <c r="Z20" s="34"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="36">
-        <v>44.0</v>
-      </c>
-      <c r="B21" s="37">
-        <v>45361.68472222222</v>
-      </c>
-      <c r="C21" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="D21" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" s="34"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="34"/>
-      <c r="P21" s="34"/>
-      <c r="Q21" s="34"/>
-      <c r="R21" s="34"/>
-      <c r="S21" s="34"/>
-      <c r="T21" s="34"/>
-      <c r="U21" s="34"/>
-      <c r="V21" s="34"/>
-      <c r="W21" s="34"/>
-      <c r="X21" s="34"/>
-      <c r="Y21" s="34"/>
-      <c r="Z21" s="34"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="31">
-        <v>45.0</v>
-      </c>
-      <c r="B22" s="32">
-        <v>45361.694444444445</v>
-      </c>
-      <c r="C22" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" s="34"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="34"/>
-      <c r="P22" s="34"/>
-      <c r="Q22" s="34"/>
-      <c r="R22" s="34"/>
-      <c r="S22" s="34"/>
-      <c r="T22" s="34"/>
-      <c r="U22" s="34"/>
-      <c r="V22" s="34"/>
-      <c r="W22" s="34"/>
-      <c r="X22" s="34"/>
-      <c r="Y22" s="34"/>
-      <c r="Z22" s="34"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="36">
-        <v>46.0</v>
-      </c>
-      <c r="B23" s="37">
-        <v>45361.70138888889</v>
-      </c>
-      <c r="C23" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="D23" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23" s="34"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
-      <c r="M23" s="34"/>
-      <c r="N23" s="34"/>
-      <c r="O23" s="34"/>
-      <c r="P23" s="34"/>
-      <c r="Q23" s="34"/>
-      <c r="R23" s="34"/>
-      <c r="S23" s="34"/>
-      <c r="T23" s="34"/>
-      <c r="U23" s="34"/>
-      <c r="V23" s="34"/>
-      <c r="W23" s="34"/>
-      <c r="X23" s="34"/>
-      <c r="Y23" s="34"/>
-      <c r="Z23" s="34"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="31">
-        <v>47.0</v>
-      </c>
-      <c r="B24" s="32">
-        <v>45362.819444444445</v>
-      </c>
-      <c r="C24" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="D24" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="E24" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" s="34"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="34"/>
-      <c r="P24" s="34"/>
-      <c r="Q24" s="34"/>
-      <c r="R24" s="34"/>
-      <c r="S24" s="34"/>
-      <c r="T24" s="34"/>
-      <c r="U24" s="34"/>
-      <c r="V24" s="34"/>
-      <c r="W24" s="34"/>
-      <c r="X24" s="34"/>
-      <c r="Y24" s="34"/>
-      <c r="Z24" s="34"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="36">
-        <v>48.0</v>
-      </c>
-      <c r="B25" s="37">
-        <v>45371.77777777778</v>
-      </c>
-      <c r="C25" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="D25" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="G25" s="34"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="34"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="34"/>
-      <c r="O25" s="34"/>
-      <c r="P25" s="34"/>
-      <c r="Q25" s="34"/>
-      <c r="R25" s="34"/>
-      <c r="S25" s="34"/>
-      <c r="T25" s="34"/>
-      <c r="U25" s="34"/>
-      <c r="V25" s="34"/>
-      <c r="W25" s="34"/>
-      <c r="X25" s="34"/>
-      <c r="Y25" s="34"/>
-      <c r="Z25" s="34"/>
+      <c r="E25" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="36"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="36"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="36"/>
+      <c r="Q25" s="36"/>
+      <c r="R25" s="36"/>
+      <c r="S25" s="36"/>
+      <c r="T25" s="36"/>
+      <c r="U25" s="36"/>
+      <c r="V25" s="36"/>
+      <c r="W25" s="36"/>
+      <c r="X25" s="36"/>
+      <c r="Y25" s="36"/>
+      <c r="Z25" s="36"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="47"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="34"/>
-      <c r="N26" s="34"/>
-      <c r="O26" s="34"/>
-      <c r="P26" s="34"/>
-      <c r="Q26" s="34"/>
-      <c r="R26" s="34"/>
-      <c r="S26" s="34"/>
-      <c r="T26" s="34"/>
-      <c r="U26" s="34"/>
-      <c r="V26" s="34"/>
-      <c r="W26" s="34"/>
-      <c r="X26" s="34"/>
-      <c r="Y26" s="34"/>
-      <c r="Z26" s="34"/>
+      <c r="A26" s="49"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="36"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="36"/>
+      <c r="Q26" s="36"/>
+      <c r="R26" s="36"/>
+      <c r="S26" s="36"/>
+      <c r="T26" s="36"/>
+      <c r="U26" s="36"/>
+      <c r="V26" s="36"/>
+      <c r="W26" s="36"/>
+      <c r="X26" s="36"/>
+      <c r="Y26" s="36"/>
+      <c r="Z26" s="36"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="31"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="34"/>
-      <c r="M27" s="34"/>
-      <c r="N27" s="34"/>
-      <c r="O27" s="34"/>
-      <c r="P27" s="34"/>
-      <c r="Q27" s="34"/>
-      <c r="R27" s="34"/>
-      <c r="S27" s="34"/>
-      <c r="T27" s="34"/>
-      <c r="U27" s="34"/>
-      <c r="V27" s="34"/>
-      <c r="W27" s="34"/>
-      <c r="X27" s="34"/>
-      <c r="Y27" s="34"/>
-      <c r="Z27" s="34"/>
+      <c r="A27" s="33"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="36"/>
+      <c r="N27" s="36"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="36"/>
+      <c r="Q27" s="36"/>
+      <c r="R27" s="36"/>
+      <c r="S27" s="36"/>
+      <c r="T27" s="36"/>
+      <c r="U27" s="36"/>
+      <c r="V27" s="36"/>
+      <c r="W27" s="36"/>
+      <c r="X27" s="36"/>
+      <c r="Y27" s="36"/>
+      <c r="Z27" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4092,37 +4113,37 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1"/>
-      <c r="F1" s="50" t="s">
-        <v>90</v>
+      <c r="A1" s="23"/>
+      <c r="F1" s="52" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1"/>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1"/>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="51" t="s">
-        <v>91</v>
+      <c r="A7" s="53" t="s">
+        <v>93</v>
       </c>
       <c r="E7" s="7">
         <v>45376.0</v>
@@ -4131,22 +4152,22 @@
     <row r="8" ht="15.75" customHeight="1"/>
     <row r="9" ht="22.5" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
@@ -4157,16 +4178,16 @@
         <v>45362.84027777778</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
@@ -4177,16 +4198,16 @@
         <v>45361.47222222222</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
@@ -4197,16 +4218,16 @@
         <v>45371.774305555555</v>
       </c>
       <c r="C12" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>68</v>
-      </c>
       <c r="E12" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
@@ -4217,16 +4238,16 @@
         <v>45362.83472222222</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1"/>
@@ -4281,112 +4302,112 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="52" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="52" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="52" t="s">
+      <c r="A1" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="C1" s="54" t="s">
         <v>12</v>
+      </c>
+      <c r="D1" s="54" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="55" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="56" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="56" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="53" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="53" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="53" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="54" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="54" t="s">
-        <v>65</v>
-      </c>
-    </row>
     <row r="11">
-      <c r="A11" s="34" t="s">
-        <v>95</v>
+      <c r="A11" s="36" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="54"/>
+      <c r="A13" s="56"/>
     </row>
     <row r="14">
-      <c r="A14" s="34"/>
+      <c r="A14" s="36"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>